<commit_message>
Updated graphic for total number of lines
</commit_message>
<xml_diff>
--- a/statistics.xlsx
+++ b/statistics.xlsx
@@ -526,312 +526,6 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>S/R</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$11:$I$11</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>Atomic</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>BEM CSS</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>BEM Flexboxgrid</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>CSS Modules</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>OOCSS</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Organic</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Raw</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>SMACSS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$15:$I$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1393757872"/>
-        <c:axId val="1374315024"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1393757872"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1374315024"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1374315024"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1393757872"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
               <c:f>Sheet1!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -1034,6 +728,345 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1369734144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Total (Number</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of lines</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Atomic</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BEM CSS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>BEM Flexboxgrid</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CSS Modules</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>OOCSS</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Organic</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Raw</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SMACSS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>324.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>283.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>260.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>297.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>290.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>342.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>288.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>288.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1342214064"/>
+        <c:axId val="1342212912"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1342214064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1342212912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1342212912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1342214064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1449,399 +1482,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Total (Number</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of lines</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Sheet1!$B$1:$I$3</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="8"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>220</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>179</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>151</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>173</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>192</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>238</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>210</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>180</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>104</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>104</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>109</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>124</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>98</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>104</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>78</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>108</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Atomic</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>BEM CSS</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>BEM Flexboxgrid</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>CSS Modules</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>OOCSS</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Organic</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Raw</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>SMACSS</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$4:$I$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>324.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>283.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>260.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>297.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>290.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>342.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>288.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>288.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1372952768"/>
-        <c:axId val="1372914080"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1372952768"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1372914080"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1372914080"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1372952768"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>HTML (File sizes)</a:t>
             </a:r>
           </a:p>
@@ -2138,7 +1778,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2469,7 +2109,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2800,7 +2440,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3106,7 +2746,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3412,7 +3052,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3670,6 +3310,312 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1348242944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S/R</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Atomic</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BEM CSS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>BEM Flexboxgrid</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CSS Modules</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>OOCSS</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Organic</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Raw</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SMACSS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$15:$I$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1393757872"/>
+        <c:axId val="1374315024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1393757872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1374315024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1374315024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1393757872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9755,36 +9701,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
@@ -9807,7 +9723,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9837,7 +9753,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9867,7 +9783,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9897,7 +9813,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9927,7 +9843,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9957,7 +9873,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9987,7 +9903,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10009,6 +9925,36 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="13" name="Chart 12"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -10291,8 +10237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix for RAW example header height
</commit_message>
<xml_diff>
--- a/statistics.xlsx
+++ b/statistics.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleshaoleg/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleshaoleg/Documents/Projects/holy-grail-markup/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -315,11 +315,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1367770176"/>
-        <c:axId val="1367739776"/>
+        <c:axId val="-1872659248"/>
+        <c:axId val="-1872657888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1367770176"/>
+        <c:axId val="-1872659248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -362,7 +362,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1367739776"/>
+        <c:crossAx val="-1872657888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -370,7 +370,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1367739776"/>
+        <c:axId val="-1872657888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -420,7 +420,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1367770176"/>
+        <c:crossAx val="-1872659248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -470,313 +470,6 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$16</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>D/R</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$11:$I$11</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>Atomic</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>BEM CSS</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>BEM Flexboxgrid</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>CSS Modules</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>OOCSS</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Organic</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Raw</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>SMACSS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$16:$I$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.54</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1369734144"/>
-        <c:axId val="1369646064"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1369734144"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1369646064"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1369646064"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1369734144"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -961,11 +654,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1342214064"/>
-        <c:axId val="1342212912"/>
+        <c:axId val="-1841790144"/>
+        <c:axId val="-1841564224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1342214064"/>
+        <c:axId val="-1841790144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1008,7 +701,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1342212912"/>
+        <c:crossAx val="-1841564224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1016,7 +709,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1342212912"/>
+        <c:axId val="-1841564224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1066,7 +759,313 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1342214064"/>
+        <c:crossAx val="-1841790144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Declarations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Atomic</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BEM CSS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>BEM Flexboxgrid</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CSS Modules</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>OOCSS</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Organic</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Raw</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SMACSS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$13:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>78.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>93.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>93.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>91.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-1845168464"/>
+        <c:axId val="-1845166144"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1845168464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1845166144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1845166144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1845168464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1292,11 +1291,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1345138064"/>
-        <c:axId val="1371702128"/>
+        <c:axId val="-1852186784"/>
+        <c:axId val="-1852184464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1345138064"/>
+        <c:axId val="-1852186784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1339,7 +1338,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1371702128"/>
+        <c:crossAx val="-1852184464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1347,7 +1346,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1371702128"/>
+        <c:axId val="-1852184464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1398,7 +1397,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1345138064"/>
+        <c:crossAx val="-1852186784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1624,11 +1623,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1348151904"/>
-        <c:axId val="1371509936"/>
+        <c:axId val="-1841499648"/>
+        <c:axId val="-1841497328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1348151904"/>
+        <c:axId val="-1841499648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1671,7 +1670,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1371509936"/>
+        <c:crossAx val="-1841497328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1679,7 +1678,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1371509936"/>
+        <c:axId val="-1841497328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1729,7 +1728,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1348151904"/>
+        <c:crossAx val="-1841499648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1955,11 +1954,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1371966864"/>
-        <c:axId val="1371968640"/>
+        <c:axId val="-1852175920"/>
+        <c:axId val="-1852173600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1371966864"/>
+        <c:axId val="-1852175920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2002,7 +2001,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1371968640"/>
+        <c:crossAx val="-1852173600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2010,7 +2009,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1371968640"/>
+        <c:axId val="-1852173600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2060,7 +2059,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1371966864"/>
+        <c:crossAx val="-1852175920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2286,11 +2285,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1392941568"/>
-        <c:axId val="1392738416"/>
+        <c:axId val="-1845411200"/>
+        <c:axId val="-1845386016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1392941568"/>
+        <c:axId val="-1845411200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2333,7 +2332,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1392738416"/>
+        <c:crossAx val="-1845386016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2341,7 +2340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1392738416"/>
+        <c:axId val="-1845386016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2391,7 +2390,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1392941568"/>
+        <c:crossAx val="-1845411200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2592,11 +2591,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1374993232"/>
-        <c:axId val="1371811056"/>
+        <c:axId val="-1844602160"/>
+        <c:axId val="-1844599840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1374993232"/>
+        <c:axId val="-1844602160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2639,7 +2638,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1371811056"/>
+        <c:crossAx val="-1844599840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2647,7 +2646,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1371811056"/>
+        <c:axId val="-1844599840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2697,7 +2696,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1374993232"/>
+        <c:crossAx val="-1844602160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2803,11 +2802,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$13</c:f>
+              <c:f>Sheet1!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Declarations</c:v>
+                  <c:v>Rules</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2856,33 +2855,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$I$13</c:f>
+              <c:f>Sheet1!$B$14:$I$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>78.0</c:v>
+                  <c:v>71.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>93.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>93.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91.0</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>93.0</c:v>
+                  <c:v>54.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>86.0</c:v>
+                  <c:v>43.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>91.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2898,11 +2897,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1368082624"/>
-        <c:axId val="1393633840"/>
+        <c:axId val="-1841478096"/>
+        <c:axId val="-1842121920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1368082624"/>
+        <c:axId val="-1841478096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2945,7 +2944,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1393633840"/>
+        <c:crossAx val="-1842121920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2953,7 +2952,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1393633840"/>
+        <c:axId val="-1842121920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3003,7 +3002,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1368082624"/>
+        <c:crossAx val="-1841478096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3109,11 +3108,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$14</c:f>
+              <c:f>Sheet1!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rules</c:v>
+                  <c:v>S/R</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3162,33 +3161,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$I$14</c:f>
+              <c:f>Sheet1!$B$15:$I$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>71.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37.0</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>54.0</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43.0</c:v>
+                  <c:v>1.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3204,11 +3203,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1348242944"/>
-        <c:axId val="1348087664"/>
+        <c:axId val="-1842177264"/>
+        <c:axId val="-1842174944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1348242944"/>
+        <c:axId val="-1842177264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3251,7 +3250,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1348087664"/>
+        <c:crossAx val="-1842174944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3259,7 +3258,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1348087664"/>
+        <c:axId val="-1842174944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3309,7 +3308,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1348242944"/>
+        <c:crossAx val="-1842177264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3415,11 +3414,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$15</c:f>
+              <c:f>Sheet1!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>S/R</c:v>
+                  <c:v>D/R</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3468,33 +3467,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$I$15</c:f>
+              <c:f>Sheet1!$B$16:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>2.54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3510,11 +3509,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1393757872"/>
-        <c:axId val="1374315024"/>
+        <c:axId val="-1957830528"/>
+        <c:axId val="-1957828208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1393757872"/>
+        <c:axId val="-1957830528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3557,7 +3556,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1374315024"/>
+        <c:crossAx val="-1957828208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3565,7 +3564,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1374315024"/>
+        <c:axId val="-1957828208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3585,6 +3584,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3615,7 +3615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1393757872"/>
+        <c:crossAx val="-1957830528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9821,36 +9821,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>47</xdr:row>
@@ -9873,7 +9843,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9903,7 +9873,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9933,7 +9903,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9955,6 +9925,36 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="14" name="Chart 13"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -10237,8 +10237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10341,35 +10341,35 @@
         <v>18</v>
       </c>
       <c r="B4" s="1">
-        <f>B2+B3</f>
+        <f t="shared" ref="B4:I4" si="0">B2+B3</f>
         <v>324</v>
       </c>
       <c r="C4" s="1">
-        <f>C2+C3</f>
+        <f t="shared" si="0"/>
         <v>283</v>
       </c>
       <c r="D4" s="1">
-        <f>D2+D3</f>
+        <f t="shared" si="0"/>
         <v>260</v>
       </c>
       <c r="E4" s="1">
-        <f>E2+E3</f>
+        <f t="shared" si="0"/>
         <v>297</v>
       </c>
       <c r="F4" s="1">
-        <f>F2+F3</f>
+        <f t="shared" si="0"/>
         <v>290</v>
       </c>
       <c r="G4" s="1">
-        <f>G2+G3</f>
+        <f t="shared" si="0"/>
         <v>342</v>
       </c>
       <c r="H4" s="1">
-        <f>H2+H3</f>
+        <f t="shared" si="0"/>
         <v>288</v>
       </c>
       <c r="I4" s="1">
-        <f>I2+I3</f>
+        <f t="shared" si="0"/>
         <v>288</v>
       </c>
     </row>
@@ -10469,27 +10469,27 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" ref="C9:H9" si="0">C7+C8</f>
+        <f t="shared" ref="C9:H9" si="1">C7+C8</f>
         <v>7.31</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.36</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.5299999999999994</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.0299999999999994</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.41</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.48</v>
       </c>
       <c r="I9" s="1">
@@ -10578,7 +10578,7 @@
         <v>93</v>
       </c>
       <c r="H13">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I13">
         <v>91</v>

</xml_diff>

<commit_message>
Updated xlsx file for statistics
</commit_message>
<xml_diff>
--- a/statistics.xlsx
+++ b/statistics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13380" yWindow="0" windowWidth="15420" windowHeight="18000" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -153,31 +153,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>HTML (Number of lines)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -220,11 +195,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$2</c:f>
+              <c:f>Sheet1!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>HTML</c:v>
+                  <c:v>Selectors</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -241,16 +216,31 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$G$1:$J$1</c:f>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>OOCSS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SMACSS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Atomic</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Organic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BEM CSS</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>BEM Flexboxgrid</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>CSS Modules</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>Raw</c:v>
                 </c:pt>
               </c:strCache>
@@ -258,18 +248,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$J$2</c:f>
+              <c:f>Sheet1!$B$12:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>108.0</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>124.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78.0</c:v>
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>79.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>48.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -285,11 +290,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-595326512"/>
-        <c:axId val="-595324192"/>
+        <c:axId val="-628697200"/>
+        <c:axId val="-628694448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-595326512"/>
+        <c:axId val="-628697200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -332,7 +337,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-595324192"/>
+        <c:crossAx val="-628694448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -340,7 +345,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-595324192"/>
+        <c:axId val="-628694448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -390,7 +395,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-595326512"/>
+        <c:crossAx val="-628697200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -474,16 +479,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Total (Number</a:t>
+              <a:t>CSS</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of lines</a:t>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> (Files sizes)</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>)</a:t>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
             </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -529,11 +537,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
+              <c:f>Sheet1!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Total</c:v>
+                  <c:v>CSS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -550,16 +558,31 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$G$1:$J$1</c:f>
+              <c:f>Sheet1!$B$6:$I$6</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>OOCSS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SMACSS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Atomic</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Organic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BEM CSS</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>BEM Flexboxgrid</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>CSS Modules</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>Raw</c:v>
                 </c:pt>
               </c:strCache>
@@ -567,18 +590,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$4:$J$4</c:f>
+              <c:f>Sheet1!$B$8:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>260.0</c:v>
+                  <c:v>2.32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>299.0</c:v>
+                  <c:v>2.373</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>288.0</c:v>
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.57</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -594,11 +632,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-595255568"/>
-        <c:axId val="-595252816"/>
+        <c:axId val="-589769776"/>
+        <c:axId val="-591923728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-595255568"/>
+        <c:axId val="-589769776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -641,7 +679,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-595252816"/>
+        <c:crossAx val="-591923728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -649,7 +687,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-595252816"/>
+        <c:axId val="-591923728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,7 +737,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-595255568"/>
+        <c:crossAx val="-589769776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -763,6 +801,1267 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Total</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> (Files sizes)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$6:$I$6</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>OOCSS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SMACSS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Atomic</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Organic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BEM CSS</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>BEM Flexboxgrid</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>CSS Modules</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Raw</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.873</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.55</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-591269920"/>
+        <c:axId val="-592437200"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-591269920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-592437200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-592437200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-591269920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rules</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>OOCSS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SMACSS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Atomic</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Organic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BEM CSS</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>BEM Flexboxgrid</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>CSS Modules</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Raw</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$14:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-664229296"/>
+        <c:axId val="-664226544"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-664229296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-664226544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-664226544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-664229296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S/R</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>OOCSS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SMACSS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Atomic</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Organic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BEM CSS</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>BEM Flexboxgrid</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>CSS Modules</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Raw</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$15:$I$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-628689088"/>
+        <c:axId val="-628686336"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-628689088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-628686336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-628686336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-628689088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>D/R</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>OOCSS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SMACSS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Atomic</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Organic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BEM CSS</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>BEM Flexboxgrid</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>CSS Modules</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Raw</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$16:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-595277088"/>
+        <c:axId val="-595275328"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-595277088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-595275328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-595275328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-595277088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -826,28 +2125,31 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$11:$I$11</c:f>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>OOCSS</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>SMACSS</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Atomic</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Organic</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>BEM CSS</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>BEM Flexboxgrid</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>CSS Modules</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Raw</c:v>
                 </c:pt>
               </c:strCache>
@@ -855,29 +2157,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$13:$I$13</c:f>
+              <c:f>Sheet1!$B$13:$I$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>93.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>91.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>78.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>93.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>94.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>101.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>94.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>85.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1048,7 +2353,338 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>HTML (Number of lines)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HTML</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>OOCSS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SMACSS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Atomic</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Organic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BEM CSS</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>BEM Flexboxgrid</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>CSS Modules</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Raw</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$I$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>98.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>108.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>104.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>104.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>108.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>124.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-593157328"/>
+        <c:axId val="-592765024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-593157328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-592765024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-592765024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-593157328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1151,16 +2787,31 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$G$1:$J$1</c:f>
+              <c:f>Sheet1!$B$1:$I$1</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>OOCSS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SMACSS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Atomic</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Organic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BEM CSS</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>BEM Flexboxgrid</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>CSS Modules</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>Raw</c:v>
                 </c:pt>
               </c:strCache>
@@ -1168,17 +2819,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$J$3</c:f>
+              <c:f>Sheet1!$B$3:$I$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>195.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>221.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>241.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>181.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>152.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>175.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>210.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1195,11 +2861,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-628763776"/>
-        <c:axId val="-628761456"/>
+        <c:axId val="-591994608"/>
+        <c:axId val="-593632448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-628763776"/>
+        <c:axId val="-591994608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1242,7 +2908,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-628761456"/>
+        <c:crossAx val="-593632448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1250,327 +2916,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-628761456"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-628763776"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>HTML (File sizes)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>HTML</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$D$6:$J$6</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Atomic</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Organic</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>BEM CSS</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>BEM Flexboxgrid</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>CSS Modules</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Raw</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$7:$J$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>6.49</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.85</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.91</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.21</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.89</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="-664248016"/>
-        <c:axId val="-628756288"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="-664248016"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-628756288"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-628756288"/>
+        <c:axId val="-593632448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1620,1246 +2966,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-664248016"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>CSS (File sizes)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>CSS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$D$6:$J$6</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Atomic</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Organic</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>BEM CSS</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>BEM Flexboxgrid</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>CSS Modules</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Raw</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$8:$J$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>2.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.57</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.96</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.45</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.57</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="-628732560"/>
-        <c:axId val="-628729808"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="-628732560"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-628729808"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-628729808"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-628732560"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Total (File sizes)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$D$6:$J$6</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Atomic</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Organic</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>BEM CSS</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>BEM Flexboxgrid</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>CSS Modules</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Raw</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$9:$J$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>9.190000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.42</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.31</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.17</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.55</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.46</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="-595306368"/>
-        <c:axId val="-595304048"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="-595306368"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-595304048"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-595304048"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-595306368"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Selectors</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$11:$I$11</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>SMACSS</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Atomic</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Organic</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>BEM CSS</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>BEM Flexboxgrid</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>CSS Modules</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Raw</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$12:$I$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>30.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>74.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>79.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>29.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>29.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>48.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="-628697200"/>
-        <c:axId val="-628694448"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="-628697200"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-628694448"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-628694448"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-628697200"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Rules</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$11:$I$11</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>SMACSS</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Atomic</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Organic</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>BEM CSS</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>BEM Flexboxgrid</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>CSS Modules</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Raw</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$14:$I$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>30.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>71.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>29.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>37.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>29.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="-664229296"/>
-        <c:axId val="-664226544"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="-664229296"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-664226544"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-664226544"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-664229296"/>
+        <c:crossAx val="-591994608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2923,6 +3030,42 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Total </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(Number of lines)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2965,11 +3108,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$15</c:f>
+              <c:f>Sheet1!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>S/R</c:v>
+                  <c:v>Total</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2986,28 +3129,31 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$11:$I$11</c:f>
+              <c:f>Sheet1!$B$1:$I$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>OOCSS</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>SMACSS</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Atomic</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Organic</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>BEM CSS</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>BEM Flexboxgrid</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>CSS Modules</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Raw</c:v>
                 </c:pt>
               </c:strCache>
@@ -3015,30 +3161,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$15:$I$15</c:f>
+              <c:f>Sheet1!$B$4:$I$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>293.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>288.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5</c:v>
+                  <c:v>325.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>345.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0</c:v>
+                  <c:v>260.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1</c:v>
+                  <c:v>299.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>288.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3054,11 +3203,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-628689088"/>
-        <c:axId val="-628686336"/>
+        <c:axId val="-594838768"/>
+        <c:axId val="-592715952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-628689088"/>
+        <c:axId val="-594838768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3101,7 +3250,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-628686336"/>
+        <c:crossAx val="-592715952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3109,7 +3258,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-628686336"/>
+        <c:axId val="-592715952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3159,7 +3308,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-628689088"/>
+        <c:crossAx val="-594838768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3223,6 +3372,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>HTML (Files sizes)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -3265,11 +3439,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$16</c:f>
+              <c:f>Sheet1!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>D/R</c:v>
+                  <c:v>HTML</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3286,28 +3460,31 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$11:$I$11</c:f>
+              <c:f>Sheet1!$B$6:$I$6</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>OOCSS</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>SMACSS</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Atomic</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Organic</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>BEM CSS</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>BEM Flexboxgrid</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>CSS Modules</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Raw</c:v>
                 </c:pt>
               </c:strCache>
@@ -3315,30 +3492,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$I$16</c:f>
+              <c:f>Sheet1!$B$7:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.56</c:v>
+                  <c:v>4.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7</c:v>
+                  <c:v>6.49</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.2</c:v>
+                  <c:v>4.85</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7</c:v>
+                  <c:v>4.91</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.2</c:v>
+                  <c:v>5.21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0</c:v>
+                  <c:v>4.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3354,11 +3534,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-595277088"/>
-        <c:axId val="-595275328"/>
+        <c:axId val="-595029648"/>
+        <c:axId val="-593374576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-595277088"/>
+        <c:axId val="-595029648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3401,7 +3581,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-595275328"/>
+        <c:crossAx val="-593374576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3409,7 +3589,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-595275328"/>
+        <c:axId val="-593374576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3429,7 +3609,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3460,7 +3639,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-595277088"/>
+        <c:crossAx val="-595029648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9486,156 +9665,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1003300</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>47</xdr:row>
@@ -9658,7 +9687,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9688,7 +9717,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9718,7 +9747,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9748,37 +9777,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="14" name="Chart 13"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9800,6 +9799,186 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Chart 14"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Chart 15"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="17" name="Chart 16"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="18" name="Chart 17"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -10082,8 +10261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:I2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C14" sqref="B14:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>